<commit_message>
increased max dose limit
</commit_message>
<xml_diff>
--- a/drl_references/raw/References.xlsx
+++ b/drl_references/raw/References.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Desktop\ct_dose_check\drl_references\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33098192-3202-4554-9140-4AAD375338EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBA11A7-4984-49C8-8B8E-154B89752AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="2" xr2:uid="{26C3E145-E6F5-9A48-AB48-8CBB735A0FEA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26C3E145-E6F5-9A48-AB48-8CBB735A0FEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Pediatric US and Europe" sheetId="1" r:id="rId1"/>
@@ -446,37 +446,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -495,6 +465,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE79AEF3-9C99-4649-A24A-52BE247D1213}">
   <dimension ref="B4:M47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:F36"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -861,295 +861,295 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="H4" s="20" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="H4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
     </row>
     <row r="5" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20" t="s">
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="20" t="s">
+      <c r="H6" s="35"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="20" t="s">
+      <c r="K6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="35" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
     </row>
     <row r="8" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="23">
+      <c r="D8" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="20">
         <v>24</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="20">
         <v>300</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="23">
+      <c r="J8" s="20">
         <v>23</v>
       </c>
-      <c r="K8" s="23">
+      <c r="K8" s="20">
         <v>344</v>
       </c>
-      <c r="L8" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="M8" s="23" t="s">
+      <c r="L8" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22" t="s">
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
     </row>
     <row r="10" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="33"/>
+      <c r="C10" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="23">
+      <c r="D10" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="20">
         <v>28</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="20">
         <v>385</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="24" t="s">
+      <c r="H10" s="33"/>
+      <c r="I10" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="23">
+      <c r="J10" s="20">
         <v>27</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="20">
         <v>440</v>
       </c>
-      <c r="L10" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="M10" s="23" t="s">
+      <c r="L10" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
     </row>
     <row r="12" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="33"/>
+      <c r="C12" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="23">
+      <c r="D12" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="20">
         <v>40</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="20">
         <v>505</v>
       </c>
-      <c r="H12" s="22"/>
-      <c r="I12" s="24" t="s">
+      <c r="H12" s="33"/>
+      <c r="I12" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="23">
+      <c r="J12" s="20">
         <v>31</v>
       </c>
-      <c r="K12" s="23">
+      <c r="K12" s="20">
         <v>518</v>
       </c>
-      <c r="L12" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="M12" s="23" t="s">
+      <c r="L12" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
     </row>
     <row r="14" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="33"/>
+      <c r="C14" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="23">
+      <c r="D14" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="20">
         <v>50</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="20">
         <v>650</v>
       </c>
-      <c r="H14" s="22"/>
-      <c r="I14" s="24" t="s">
+      <c r="H14" s="33"/>
+      <c r="I14" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="23">
+      <c r="J14" s="20">
         <v>55</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="20">
         <v>910</v>
       </c>
-      <c r="L14" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="M14" s="23" t="s">
+      <c r="L14" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M14" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="20">
         <v>35</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="30" t="s">
         <v>54</v>
       </c>
       <c r="I16" s="3"/>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26" t="s">
+      <c r="K16" s="32"/>
+      <c r="L16" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="M16" s="26"/>
+      <c r="M16" s="32"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="H17" s="25"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="H17" s="30"/>
       <c r="I17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1167,180 +1167,180 @@
       </c>
     </row>
     <row r="18" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="25"/>
-      <c r="C18" s="25" t="s">
+      <c r="B18" s="30"/>
+      <c r="C18" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="20">
         <v>50</v>
       </c>
-      <c r="H18" s="25"/>
-      <c r="I18" s="27" t="s">
+      <c r="H18" s="30"/>
+      <c r="I18" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="23">
+      <c r="J18" s="20">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K18" s="23">
+      <c r="K18" s="20">
         <v>49</v>
       </c>
-      <c r="L18" s="23">
+      <c r="L18" s="20">
         <v>2.4</v>
       </c>
-      <c r="M18" s="23">
+      <c r="M18" s="20">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
     </row>
     <row r="20" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="25"/>
-      <c r="C20" s="25" t="s">
+      <c r="B20" s="30"/>
+      <c r="C20" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="20">
         <v>70</v>
       </c>
-      <c r="H20" s="25"/>
-      <c r="I20" s="27" t="s">
+      <c r="H20" s="30"/>
+      <c r="I20" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="J20" s="23">
+      <c r="J20" s="20">
         <v>2.5</v>
       </c>
-      <c r="K20" s="23">
+      <c r="K20" s="20">
         <v>70</v>
       </c>
-      <c r="L20" s="23">
+      <c r="L20" s="20">
         <v>2.9</v>
       </c>
-      <c r="M20" s="23">
+      <c r="M20" s="20">
         <v>95</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
     </row>
     <row r="22" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="25"/>
-      <c r="C22" s="25" t="s">
+      <c r="B22" s="30"/>
+      <c r="C22" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="20">
         <v>115</v>
       </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="27" t="s">
+      <c r="H22" s="30"/>
+      <c r="I22" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="J22" s="23">
+      <c r="J22" s="20">
         <v>4.0999999999999996</v>
       </c>
-      <c r="K22" s="23">
+      <c r="K22" s="20">
         <v>128</v>
       </c>
-      <c r="L22" s="23">
+      <c r="L22" s="20">
         <v>7.2</v>
       </c>
-      <c r="M22" s="23">
+      <c r="M22" s="20">
         <v>272</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
     </row>
     <row r="24" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="25"/>
-      <c r="C24" s="25" t="s">
+      <c r="B24" s="30"/>
+      <c r="C24" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="20">
         <v>200</v>
       </c>
-      <c r="H24" s="25"/>
-      <c r="I24" s="27" t="s">
+      <c r="H24" s="30"/>
+      <c r="I24" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="J24" s="23">
+      <c r="J24" s="20">
         <v>7.4</v>
       </c>
-      <c r="K24" s="23">
+      <c r="K24" s="20">
         <v>257</v>
       </c>
-      <c r="L24" s="23">
+      <c r="L24" s="20">
         <v>14</v>
       </c>
-      <c r="M24" s="23">
+      <c r="M24" s="20">
         <v>596</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
     </row>
     <row r="26" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="28" t="s">
@@ -1352,28 +1352,28 @@
       <c r="D26" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="23">
+      <c r="E26" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="20">
         <v>45</v>
       </c>
       <c r="H26" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="I26" s="30" t="s">
+      <c r="I26" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J26" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="K26" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="L26" s="23">
+      <c r="J26" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="K26" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="L26" s="20">
         <v>2.4</v>
       </c>
-      <c r="M26" s="23">
+      <c r="M26" s="20">
         <v>60</v>
       </c>
     </row>
@@ -1381,14 +1381,14 @@
       <c r="B27" s="28"/>
       <c r="C27" s="28"/>
       <c r="D27" s="28"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="23"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="20"/>
       <c r="H27" s="28"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
     </row>
     <row r="28" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="28"/>
@@ -1398,26 +1398,26 @@
       <c r="D28" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="20">
         <v>120</v>
       </c>
       <c r="H28" s="28"/>
-      <c r="I28" s="30" t="s">
+      <c r="I28" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="J28" s="23">
+      <c r="J28" s="20">
         <v>2.6</v>
       </c>
-      <c r="K28" s="23">
+      <c r="K28" s="20">
         <v>95</v>
       </c>
-      <c r="L28" s="23">
+      <c r="L28" s="20">
         <v>2.9</v>
       </c>
-      <c r="M28" s="23">
+      <c r="M28" s="20">
         <v>100</v>
       </c>
     </row>
@@ -1425,14 +1425,14 @@
       <c r="B29" s="28"/>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
       <c r="H29" s="28"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
     </row>
     <row r="30" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="28"/>
@@ -1442,26 +1442,26 @@
       <c r="D30" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="23">
+      <c r="F30" s="20">
         <v>150</v>
       </c>
       <c r="H30" s="28"/>
-      <c r="I30" s="30" t="s">
+      <c r="I30" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="23">
+      <c r="J30" s="20">
         <v>4.8</v>
       </c>
-      <c r="K30" s="23">
+      <c r="K30" s="20">
         <v>171</v>
       </c>
-      <c r="L30" s="23">
+      <c r="L30" s="20">
         <v>4.5999999999999996</v>
       </c>
-      <c r="M30" s="23">
+      <c r="M30" s="20">
         <v>170</v>
       </c>
     </row>
@@ -1469,14 +1469,14 @@
       <c r="B31" s="28"/>
       <c r="C31" s="28"/>
       <c r="D31" s="28"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
       <c r="H31" s="28"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
     </row>
     <row r="32" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="28"/>
@@ -1486,26 +1486,26 @@
       <c r="D32" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="20">
         <v>210</v>
       </c>
       <c r="H32" s="28"/>
-      <c r="I32" s="30" t="s">
+      <c r="I32" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J32" s="23">
+      <c r="J32" s="20">
         <v>8.1</v>
       </c>
-      <c r="K32" s="23">
+      <c r="K32" s="20">
         <v>367</v>
       </c>
-      <c r="L32" s="23">
+      <c r="L32" s="20">
         <v>7.9</v>
       </c>
-      <c r="M32" s="23">
+      <c r="M32" s="20">
         <v>358</v>
       </c>
     </row>
@@ -1513,14 +1513,14 @@
       <c r="B33" s="28"/>
       <c r="C33" s="28"/>
       <c r="D33" s="28"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
       <c r="H33" s="28"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
     </row>
     <row r="34" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="28"/>
@@ -1530,26 +1530,26 @@
       <c r="D34" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="20">
         <v>13</v>
       </c>
-      <c r="F34" s="23">
-        <v>48</v>
+      <c r="F34" s="20">
+        <v>480</v>
       </c>
       <c r="H34" s="28"/>
-      <c r="I34" s="30" t="s">
+      <c r="I34" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="J34" s="23">
+      <c r="J34" s="20">
         <v>11</v>
       </c>
-      <c r="K34" s="23">
+      <c r="K34" s="20">
         <v>510</v>
       </c>
-      <c r="L34" s="23">
+      <c r="L34" s="20">
         <v>11</v>
       </c>
-      <c r="M34" s="23">
+      <c r="M34" s="20">
         <v>511</v>
       </c>
     </row>
@@ -1557,179 +1557,326 @@
       <c r="B35" s="28"/>
       <c r="C35" s="28"/>
       <c r="D35" s="28"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
       <c r="H35" s="28"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="C36" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="H36" s="36" t="s">
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="H36" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="I36" s="35" t="s">
+      <c r="I36" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="J36" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="K36" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="L36" s="29">
+      <c r="J36" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="K36" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="L36" s="27">
         <v>2.7</v>
       </c>
-      <c r="M36" s="29">
+      <c r="M36" s="27">
         <v>89</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H37" s="36"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H38" s="36"/>
-      <c r="I38" s="35" t="s">
+      <c r="H38" s="26"/>
+      <c r="I38" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="J38" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="K38" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="L38" s="23">
+      <c r="J38" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="K38" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="L38" s="20">
         <v>3</v>
       </c>
-      <c r="M38" s="23">
+      <c r="M38" s="20">
         <v>109</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H39" s="36"/>
-      <c r="I39" s="35"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="23"/>
-      <c r="M39" s="23"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H40" s="36"/>
-      <c r="I40" s="35" t="s">
+      <c r="H40" s="26"/>
+      <c r="I40" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="J40" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="K40" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="L40" s="23">
+      <c r="J40" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="K40" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="L40" s="20">
         <v>4.3</v>
       </c>
-      <c r="M40" s="23">
+      <c r="M40" s="20">
         <v>204</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H41" s="36"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="23"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="23"/>
-      <c r="M41" s="23"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H42" s="36"/>
-      <c r="I42" s="35" t="s">
+      <c r="H42" s="26"/>
+      <c r="I42" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="J42" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="K42" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="L42" s="23">
+      <c r="J42" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="K42" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="L42" s="20">
         <v>9.1</v>
       </c>
-      <c r="M42" s="23">
+      <c r="M42" s="20">
         <v>437</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H43" s="36"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="23"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="23"/>
-      <c r="M43" s="23"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H44" s="36"/>
-      <c r="I44" s="35" t="s">
+      <c r="H44" s="26"/>
+      <c r="I44" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="J44" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="K44" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="L44" s="23">
+      <c r="J44" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="K44" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="L44" s="20">
         <v>17</v>
       </c>
-      <c r="M44" s="23">
+      <c r="M44" s="20">
         <v>964</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H45" s="36"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="23"/>
-      <c r="M45" s="23"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="20"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.3">
       <c r="H46" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I46" s="31" t="s">
+      <c r="I46" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31"/>
-      <c r="M46" s="31"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="I47" s="33" t="s">
+      <c r="I47" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="J47" s="34"/>
-      <c r="K47" s="34"/>
-      <c r="L47" s="34"/>
-      <c r="M47" s="34"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="24"/>
+      <c r="L47" s="24"/>
+      <c r="M47" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="171">
+    <mergeCell ref="B4:F5"/>
+    <mergeCell ref="H4:M5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H15"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="B16:B25"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="H16:H25"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="H26:H35"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="M34:M35"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="K44:K45"/>
+    <mergeCell ref="L44:L45"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="L34:L35"/>
     <mergeCell ref="K38:K39"/>
     <mergeCell ref="L38:L39"/>
     <mergeCell ref="J40:J41"/>
@@ -1754,153 +1901,6 @@
     <mergeCell ref="K42:K43"/>
     <mergeCell ref="L42:L43"/>
     <mergeCell ref="J44:J45"/>
-    <mergeCell ref="K44:K45"/>
-    <mergeCell ref="L44:L45"/>
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="M34:M35"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="M32:M33"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="B26:B35"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="H26:H35"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="B16:B25"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="H16:H25"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:H15"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="B4:F5"/>
-    <mergeCell ref="H4:M5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C36" r:id="rId1" xr:uid="{487C8AC2-6339-F147-BAAA-9B2E7368D60F}"/>
@@ -2218,7 +2218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2769BF2C-A4D0-1F46-B0E6-F86F7143B7EE}">
   <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="21" t="s">
         <v>63</v>
       </c>
       <c r="D15" s="44"/>
@@ -2466,11 +2466,11 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>